<commit_message>
Add U_DC_PE, U_DC_NE, and WATER_DEPTH
</commit_message>
<xml_diff>
--- a/import-specification/devices/inverter.xlsx
+++ b/import-specification/devices/inverter.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11109"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albert/Project/mc/safersun/import-specification-generator/meteocontrol.github.com/import-specification/devices/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24016BB-C0CB-AE43-9FD7-6BD6CC68E8B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="128">
   <si>
     <t>Field Type</t>
   </si>
@@ -365,6 +370,12 @@
     <t>Voltage DC (single input or accumulated)</t>
   </si>
   <si>
+    <t>U_DC_NE</t>
+  </si>
+  <si>
+    <t>U_DC_PE</t>
+  </si>
+  <si>
     <t>STATE[1..x]</t>
   </si>
   <si>
@@ -387,31 +398,43 @@
   </si>
   <si>
     <t>Telegrams received (communication quality)</t>
+  </si>
+  <si>
+    <t>Voltage DC negative pole to earth</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Voltage DC positive pole to earth</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Wawati TC"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -419,31 +442,41 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -733,29 +766,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:H46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.424561" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="22.280273" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="54.129639" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="37.705078" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -781,7 +810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -801,7 +830,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -824,7 +853,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -844,7 +873,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -861,7 +890,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -878,7 +907,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -895,7 +924,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -912,7 +941,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -929,7 +958,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -946,7 +975,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -957,7 +986,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -968,7 +997,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -979,7 +1008,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -990,7 +1019,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1001,7 +1030,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1015,7 +1044,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1029,7 +1058,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1043,7 +1072,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1057,7 +1086,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1071,7 +1100,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1085,7 +1114,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1099,7 +1128,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1113,7 +1142,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1127,7 +1156,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1141,7 +1170,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -1155,7 +1184,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1169,7 +1198,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1183,7 +1212,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -1197,7 +1226,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1214,7 +1243,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -1228,7 +1257,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1242,7 +1271,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -1256,7 +1285,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1270,7 +1299,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1284,7 +1313,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1298,7 +1327,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1312,7 +1341,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1326,7 +1355,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1340,7 +1369,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1354,7 +1383,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -1368,7 +1397,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>38</v>
       </c>
@@ -1382,62 +1411,82 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>38</v>
       </c>
       <c r="B43" t="s">
         <v>116</v>
       </c>
-      <c r="D43" t="s">
+      <c r="C43" t="s">
+        <v>106</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
+        <v>106</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" t="s">
         <v>118</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
-      <c r="A45" t="s">
-        <v>38</v>
-      </c>
-      <c r="B45" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" t="s">
         <v>120</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
-      <c r="A46" t="s">
-        <v>38</v>
-      </c>
-      <c r="B46" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" t="s">
         <v>122</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>123</v>
       </c>
     </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" t="s">
+        <v>124</v>
+      </c>
+      <c r="D48" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update description of inverter abbreviations
</commit_message>
<xml_diff>
--- a/import-specification/devices/inverter.xlsx
+++ b/import-specification/devices/inverter.xlsx
@@ -230,13 +230,13 @@
     <t>I_DC[1..x]</t>
   </si>
   <si>
-    <t>Current DC (single input or accumulated)</t>
+    <t>Current DC MPPT x</t>
   </si>
   <si>
     <t>I_DC[1..x]_[1..x]</t>
   </si>
   <si>
-    <t>Current DC (single string)</t>
+    <t>Current DC MPPT x Input x</t>
   </si>
   <si>
     <t>I_GDFI</t>
@@ -272,7 +272,7 @@
     <t>P_DC[1..x]</t>
   </si>
   <si>
-    <t>Power DC (single input or accumulated)</t>
+    <t>Power DC MPPT x</t>
   </si>
   <si>
     <t>Q_AC[1..3]</t>
@@ -353,13 +353,13 @@
     <t>U_DC[1..x]</t>
   </si>
   <si>
-    <t>Voltage DC (single input or accumulated)</t>
+    <t>Voltage DC MPPT x</t>
   </si>
   <si>
     <t>U_DC[1..x]_[1..x]</t>
   </si>
   <si>
-    <t>Voltage DC (single string)</t>
+    <t>Voltage DC MPPT x Input x</t>
   </si>
   <si>
     <t>U_DC_NE</t>

</xml_diff>